<commit_message>
Added column "mX0" (derived from cX0) to metadata
</commit_message>
<xml_diff>
--- a/BacillusDaten/Stamm185/metadata.xlsx
+++ b/BacillusDaten/Stamm185/metadata.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="V:\biomoni\BacillusDaten\Stamm185\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63F07243-D59F-4C08-A4BD-18E18DB7DAAD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56A579D4-DE2A-4AD5-86A6-DF0ACFE190F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="1620" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="37">
   <si>
     <t>Experiment</t>
   </si>
@@ -142,6 +142,9 @@
   </si>
   <si>
     <t>mg/L</t>
+  </si>
+  <si>
+    <t>mX0</t>
   </si>
 </sst>
 </file>
@@ -516,10 +519,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:S9"/>
+  <dimension ref="A1:T9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8:XFD9"/>
+      <selection activeCell="I1" sqref="I1:I1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -527,15 +530,15 @@
     <col min="1" max="1" width="11.28515625" bestFit="1" customWidth="1"/>
     <col min="2" max="6" width="18.85546875" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="8.7109375" customWidth="1"/>
-    <col min="8" max="8" width="11" customWidth="1"/>
-    <col min="9" max="9" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="9.85546875" customWidth="1"/>
-    <col min="11" max="11" width="13.5703125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="9.140625" style="5"/>
-    <col min="18" max="18" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="11" customWidth="1"/>
+    <col min="10" max="10" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="9.85546875" customWidth="1"/>
+    <col min="12" max="12" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="9.140625" style="5"/>
+    <col min="19" max="19" width="11.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -561,40 +564,43 @@
         <v>4</v>
       </c>
       <c r="I1" t="s">
+        <v>36</v>
+      </c>
+      <c r="J1" t="s">
         <v>5</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>6</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>23</v>
       </c>
-      <c r="L1" s="5" t="s">
+      <c r="M1" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="M1" s="5" t="s">
+      <c r="N1" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
         <v>7</v>
       </c>
-      <c r="O1" t="s">
+      <c r="P1" t="s">
         <v>8</v>
       </c>
-      <c r="P1" t="s">
+      <c r="Q1" t="s">
         <v>9</v>
       </c>
-      <c r="Q1" s="5" t="s">
+      <c r="R1" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="R1" s="8" t="s">
+      <c r="S1" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="S1" s="2" t="s">
+      <c r="T1" s="2" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>21</v>
       </c>
@@ -617,38 +623,41 @@
         <v>24</v>
       </c>
       <c r="I2" t="s">
+        <v>25</v>
+      </c>
+      <c r="J2" t="s">
         <v>24</v>
       </c>
-      <c r="J2" t="s">
+      <c r="K2" t="s">
         <v>25</v>
       </c>
-      <c r="K2" t="s">
+      <c r="L2" t="s">
         <v>27</v>
       </c>
-      <c r="L2" s="5" t="s">
+      <c r="M2" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="M2" s="5" t="s">
+      <c r="N2" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="N2" t="s">
+      <c r="O2" t="s">
         <v>24</v>
       </c>
-      <c r="O2" t="s">
+      <c r="P2" t="s">
         <v>26</v>
       </c>
-      <c r="P2" t="s">
+      <c r="Q2" t="s">
         <v>30</v>
       </c>
-      <c r="Q2" s="5" t="s">
+      <c r="R2" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="R2" s="8" t="s">
+      <c r="S2" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="S2" s="2"/>
+      <c r="T2" s="2"/>
     </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>13</v>
       </c>
@@ -673,42 +682,46 @@
       <c r="H3" s="10">
         <v>0.02</v>
       </c>
-      <c r="I3" s="9">
+      <c r="I3" s="10">
+        <f>H3*0.5</f>
+        <v>0.01</v>
+      </c>
+      <c r="J3" s="9">
         <v>27.560040253447639</v>
       </c>
-      <c r="J3" s="11">
-        <f>I3*0.5</f>
+      <c r="K3" s="11">
+        <f>J3*0.5</f>
         <v>13.780020126723819</v>
       </c>
-      <c r="K3">
+      <c r="L3">
         <v>0.3669</v>
       </c>
-      <c r="L3" s="5">
+      <c r="M3" s="5">
         <v>8.6400000000000005E-2</v>
       </c>
-      <c r="M3" s="5">
+      <c r="N3" s="5">
         <v>1.1399999999999999</v>
       </c>
-      <c r="N3" s="9">
+      <c r="O3" s="9">
         <v>150</v>
       </c>
-      <c r="O3">
+      <c r="P3">
         <v>0.5</v>
       </c>
-      <c r="P3">
+      <c r="Q3">
         <v>37</v>
       </c>
-      <c r="Q3" s="5">
+      <c r="R3" s="5">
         <v>184.61</v>
       </c>
-      <c r="R3" s="5">
+      <c r="S3" s="5">
         <v>0</v>
       </c>
-      <c r="S3" t="s">
+      <c r="T3" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>14</v>
       </c>
@@ -733,42 +746,46 @@
       <c r="H4" s="10">
         <v>3.5999999999999997E-2</v>
       </c>
-      <c r="I4" s="9">
+      <c r="I4" s="10">
+        <f t="shared" ref="I4:K7" si="0">H4*0.5</f>
+        <v>1.7999999999999999E-2</v>
+      </c>
+      <c r="J4" s="9">
         <v>19.608350430319199</v>
       </c>
-      <c r="J4" s="11">
-        <f t="shared" ref="J4:J9" si="0">I4*0.5</f>
+      <c r="K4" s="11">
+        <f t="shared" si="0"/>
         <v>9.8041752151595993</v>
       </c>
-      <c r="K4">
+      <c r="L4">
         <v>0.3669</v>
       </c>
-      <c r="L4" s="5">
+      <c r="M4" s="5">
         <v>8.6400000000000005E-2</v>
       </c>
-      <c r="M4" s="5">
+      <c r="N4" s="5">
         <v>1.1399999999999999</v>
       </c>
-      <c r="N4" s="9">
+      <c r="O4" s="9">
         <v>150</v>
       </c>
-      <c r="O4">
+      <c r="P4">
         <v>0.5</v>
       </c>
-      <c r="P4">
+      <c r="Q4">
         <v>37</v>
       </c>
-      <c r="Q4" s="5">
+      <c r="R4" s="5">
         <v>184.61</v>
       </c>
-      <c r="R4" s="5">
+      <c r="S4" s="5">
         <v>5.24</v>
       </c>
-      <c r="S4" t="s">
+      <c r="T4" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>15</v>
       </c>
@@ -793,42 +810,46 @@
       <c r="H5" s="10">
         <v>8.0057580000000003E-2</v>
       </c>
-      <c r="I5" s="9">
+      <c r="I5" s="10">
+        <f t="shared" si="0"/>
+        <v>4.0028790000000002E-2</v>
+      </c>
+      <c r="J5" s="9">
         <v>27.369118762743817</v>
       </c>
-      <c r="J5" s="11">
+      <c r="K5" s="11">
         <f t="shared" si="0"/>
         <v>13.684559381371908</v>
       </c>
-      <c r="K5">
+      <c r="L5">
         <v>0.3669</v>
       </c>
-      <c r="L5" s="5">
+      <c r="M5" s="5">
         <v>8.6400000000000005E-2</v>
       </c>
-      <c r="M5" s="5">
+      <c r="N5" s="5">
         <v>1.1399999999999999</v>
       </c>
-      <c r="N5" s="9">
+      <c r="O5" s="9">
         <v>303.51</v>
       </c>
-      <c r="O5">
+      <c r="P5">
         <v>0.5</v>
       </c>
-      <c r="P5">
+      <c r="Q5">
         <v>37</v>
       </c>
-      <c r="Q5" s="5">
+      <c r="R5" s="5">
         <v>184.61</v>
       </c>
-      <c r="R5" s="9">
+      <c r="S5" s="9">
         <v>1.0241379310344827</v>
       </c>
-      <c r="S5" t="s">
+      <c r="T5" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>10</v>
       </c>
@@ -853,42 +874,46 @@
       <c r="H6" s="10">
         <v>4.3771169999999998E-2</v>
       </c>
-      <c r="I6" s="9">
+      <c r="I6" s="10">
+        <f t="shared" si="0"/>
+        <v>2.1885584999999999E-2</v>
+      </c>
+      <c r="J6" s="9">
         <v>32.781673628850491</v>
       </c>
-      <c r="J6" s="11">
+      <c r="K6" s="11">
         <f t="shared" si="0"/>
         <v>16.390836814425246</v>
       </c>
-      <c r="K6">
+      <c r="L6">
         <v>0.3669</v>
       </c>
-      <c r="L6" s="5">
+      <c r="M6" s="5">
         <v>8.6400000000000005E-2</v>
       </c>
-      <c r="M6" s="5">
+      <c r="N6" s="5">
         <v>1.1399999999999999</v>
       </c>
-      <c r="N6" s="9">
+      <c r="O6" s="9">
         <v>335.72072126220888</v>
       </c>
-      <c r="O6">
+      <c r="P6">
         <v>0.5</v>
       </c>
-      <c r="P6">
+      <c r="Q6">
         <v>37</v>
       </c>
-      <c r="Q6" s="5">
+      <c r="R6" s="5">
         <v>184.61</v>
       </c>
-      <c r="R6" s="16">
+      <c r="S6" s="16">
         <v>10.6206896551724</v>
       </c>
-      <c r="S6" t="s">
+      <c r="T6" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="7" spans="1:19" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:20" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>11</v>
       </c>
@@ -913,68 +938,74 @@
       <c r="H7" s="15">
         <v>5.3897609999999999E-2</v>
       </c>
-      <c r="I7" s="14">
+      <c r="I7" s="15">
+        <f t="shared" si="0"/>
+        <v>2.6948804999999999E-2</v>
+      </c>
+      <c r="J7" s="14">
         <v>30.541769797145008</v>
       </c>
-      <c r="J7" s="12">
+      <c r="K7" s="12">
         <f t="shared" si="0"/>
         <v>15.270884898572504</v>
       </c>
-      <c r="K7" s="3">
+      <c r="L7" s="3">
         <v>0.3669</v>
       </c>
-      <c r="L7" s="6">
+      <c r="M7" s="6">
         <v>8.6400000000000005E-2</v>
       </c>
-      <c r="M7" s="6">
+      <c r="N7" s="6">
         <v>1.1399999999999999</v>
       </c>
-      <c r="N7" s="14">
+      <c r="O7" s="14">
         <v>336.59095416979716</v>
       </c>
-      <c r="O7" s="3">
+      <c r="P7" s="3">
         <v>0.5</v>
       </c>
-      <c r="P7" s="3">
+      <c r="Q7" s="3">
         <v>37</v>
       </c>
-      <c r="Q7" s="6">
+      <c r="R7" s="6">
         <v>184.61</v>
       </c>
-      <c r="R7" s="9">
+      <c r="S7" s="9">
         <v>0.44137931034482758</v>
       </c>
-      <c r="S7" t="s">
+      <c r="T7" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
       <c r="D8" s="1"/>
       <c r="E8" s="13"/>
       <c r="F8" s="1"/>
       <c r="H8" s="10"/>
-      <c r="I8" s="9"/>
-      <c r="J8" s="11"/>
-      <c r="N8" s="9"/>
-      <c r="P8" s="7"/>
-      <c r="Q8" s="5"/>
-      <c r="R8" s="17"/>
+      <c r="I8" s="10"/>
+      <c r="J8" s="9"/>
+      <c r="K8" s="11"/>
+      <c r="O8" s="9"/>
+      <c r="Q8" s="7"/>
+      <c r="R8" s="5"/>
+      <c r="S8" s="17"/>
     </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:20" x14ac:dyDescent="0.25">
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
       <c r="D9" s="1"/>
       <c r="E9" s="1"/>
       <c r="F9" s="1"/>
       <c r="H9" s="10"/>
-      <c r="I9" s="9"/>
-      <c r="J9" s="11"/>
-      <c r="N9" s="9"/>
-      <c r="P9" s="7"/>
-      <c r="Q9" s="5"/>
-      <c r="R9" s="17"/>
+      <c r="I9" s="10"/>
+      <c r="J9" s="9"/>
+      <c r="K9" s="11"/>
+      <c r="O9" s="9"/>
+      <c r="Q9" s="7"/>
+      <c r="R9" s="5"/>
+      <c r="S9" s="17"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>